<commit_message>
Author : Rachit Goyal File Modified : RachitGoyal.xlsx Reviewed by : Ruchi Pareek
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/RachitGoyal.xlsx
+++ b/TeamDetails/TasksBreakDown/RachitGoyal.xlsx
@@ -27,8 +27,114 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Rachit Goyal</author>
+  </authors>
+  <commentList>
+    <comment ref="G23" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rachit Goyal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Time estimation for the above Story.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G38" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rachit Goyal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Time estimation for the above Story.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G55" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rachit Goyal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Time estimation for the above Story.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G56" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rachit Goyal:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Total time Estimation of all the Stories.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="52">
   <si>
     <t>Story ID</t>
   </si>
@@ -75,53 +181,6 @@
     <t xml:space="preserve">Understand the bigger picture of the story. (Why Part ???)                                                          To provide a search feature for Batch and details regarding the Batch </t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Create a table using </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Angular U-grid</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. For  the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Display of information</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>SSDMS - 62</t>
   </si>
   <si>
@@ -157,7 +216,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Create </t>
+      <t>Create a Downlaod</t>
     </r>
     <r>
       <rPr>
@@ -168,7 +227,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Search field</t>
+      <t xml:space="preserve"> Button</t>
     </r>
     <r>
       <rPr>
@@ -178,7 +237,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> &amp; </t>
+      <t>.(certificate)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create a </t>
     </r>
     <r>
       <rPr>
@@ -189,7 +253,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Search button</t>
+      <t>Block Diagram</t>
     </r>
     <r>
       <rPr>
@@ -204,7 +268,7 @@
   </si>
   <si>
     <r>
-      <t>Create the connection between the</t>
+      <t>Create a</t>
     </r>
     <r>
       <rPr>
@@ -215,7 +279,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Table</t>
+      <t xml:space="preserve"> Block Diagram</t>
     </r>
     <r>
       <rPr>
@@ -225,7 +289,159 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> and </t>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pick </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Batch ID</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Front-end</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>searching.</t>
+    </r>
+  </si>
+  <si>
+    <t>T-7</t>
+  </si>
+  <si>
+    <t>T-8</t>
+  </si>
+  <si>
+    <t>T-9</t>
+  </si>
+  <si>
+    <t>T-10</t>
+  </si>
+  <si>
+    <t>T-11</t>
+  </si>
+  <si>
+    <t>T-12</t>
+  </si>
+  <si>
+    <t>T-13</t>
+  </si>
+  <si>
+    <t>T-14</t>
+  </si>
+  <si>
+    <r>
+      <t>Send</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Batch ID</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Back-end</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Receive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> data from </t>
     </r>
     <r>
       <rPr>
@@ -251,7 +467,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Create connection between </t>
+      <t xml:space="preserve">Implement Database </t>
     </r>
     <r>
       <rPr>
@@ -262,7 +478,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Front-end</t>
+      <t>SQL queries</t>
     </r>
     <r>
       <rPr>
@@ -272,7 +488,194 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> &amp; </t>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Receive data sent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> by </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Database</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SQL query</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Send</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> data to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>frontend</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Receive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> detail of</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Batch ID.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Populate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the table with data</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> received</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
     </r>
     <r>
       <rPr>
@@ -298,7 +701,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Create </t>
+      <t xml:space="preserve">Unit </t>
     </r>
     <r>
       <rPr>
@@ -309,49 +712,105 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Back-end</t>
-    </r>
+      <t>Testing.</t>
+    </r>
+  </si>
+  <si>
+    <t>Debugging.</t>
+  </si>
+  <si>
+    <t>Code Review</t>
+  </si>
+  <si>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> using </t>
+      <t>Import</t>
     </r>
     <r>
       <rPr>
-        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Java</t>
-    </r>
+      <t xml:space="preserve"> (window).</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> and </t>
+      <t>Analysis</t>
     </r>
     <r>
       <rPr>
-        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Springboot</t>
+      <t xml:space="preserve"> (Create layout for search so that user can search).</t>
+    </r>
+  </si>
+  <si>
+    <t>Analysis (Create layout for search so that user can search).</t>
+  </si>
+  <si>
+    <t>T-15</t>
+  </si>
+  <si>
+    <t>T-16</t>
+  </si>
+  <si>
+    <t>T-17</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Store</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the link of the file on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Database</t>
     </r>
     <r>
       <rPr>
@@ -366,9 +825,6 @@
   </si>
   <si>
     <r>
-      <t>Create a Downlaod</t>
-    </r>
-    <r>
       <rPr>
         <b/>
         <sz val="11"/>
@@ -377,7 +833,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Button</t>
+      <t>Store</t>
     </r>
     <r>
       <rPr>
@@ -387,12 +843,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>.(certificate)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Create a </t>
+      <t xml:space="preserve"> the file on the </t>
     </r>
     <r>
       <rPr>
@@ -403,7 +854,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Block Diagram</t>
+      <t>Database</t>
     </r>
     <r>
       <rPr>
@@ -415,160 +866,13 @@
       </rPr>
       <t>.</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Create connection between </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Front-end</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> &amp; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Back-end.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Unit Testing</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> &amp; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Debugging.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Create </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Textbox</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> &amp; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Search button</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Create a</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Block Diagram</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>Unit Testing &amp; Debugging.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -600,8 +904,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -652,12 +988,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFFF7C80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -788,11 +1130,139 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -813,9 +1283,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -836,20 +1303,99 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -878,8 +1424,20 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -905,12 +1463,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -920,28 +1472,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -970,8 +1501,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF7C80"/>
+      <color rgb="FFFF3300"/>
       <color rgb="FFCC6600"/>
-      <color rgb="FFFF7C80"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1247,11 +1779,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,706 +1820,1231 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="34"/>
+      <c r="A3" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="64"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="37"/>
+      <c r="A4" s="65"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="67"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="24">
-        <f>SUM(G5:G11)</f>
-        <v>20</v>
-      </c>
-      <c r="C5" s="22" t="s">
+      <c r="A5" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="50">
+        <f>SUM(E5:E22)</f>
+        <v>23</v>
+      </c>
+      <c r="C5" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="57" t="s">
+      <c r="D5" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="53">
-        <v>2</v>
-      </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="55">
+      <c r="E5" s="74">
+        <v>1</v>
+      </c>
+      <c r="F5" s="48">
+        <v>0</v>
+      </c>
+      <c r="G5" s="76">
         <f>E5-F5</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="56"/>
+      <c r="A6" s="54"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="77"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="25"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="51"/>
       <c r="C7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="19">
-        <v>1</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="21">
-        <f t="shared" ref="G7:G30" si="0">E7-F7</f>
-        <v>1</v>
+      <c r="D7" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="21">
+        <v>2</v>
+      </c>
+      <c r="F7" s="19">
+        <v>0</v>
+      </c>
+      <c r="G7" s="18">
+        <f t="shared" ref="G7:G17" si="0">E7-F7</f>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="25"/>
+      <c r="A8" s="54"/>
+      <c r="B8" s="51"/>
       <c r="C8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="19">
-        <v>2</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="21">
-        <f t="shared" si="0"/>
-        <v>2</v>
+      <c r="D8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="17">
+        <v>1</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0</v>
+      </c>
+      <c r="G8" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="25"/>
+      <c r="A9" s="54"/>
+      <c r="B9" s="51"/>
       <c r="C9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="19">
-        <v>8</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="21">
-        <f t="shared" si="0"/>
-        <v>8</v>
+      <c r="D9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="17">
+        <v>1</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0</v>
+      </c>
+      <c r="G9" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="6" t="s">
+      <c r="A10" s="54"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="19">
-        <v>4</v>
-      </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="21">
-        <f t="shared" si="0"/>
-        <v>4</v>
+      <c r="D10" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="17">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0</v>
+      </c>
+      <c r="G10" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
-      <c r="B11" s="26"/>
+      <c r="A11" s="54"/>
+      <c r="B11" s="51"/>
       <c r="C11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="17">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0</v>
+      </c>
+      <c r="G11" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="54"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="17">
+        <v>1</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0</v>
+      </c>
+      <c r="G12" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="54"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="17">
+        <v>1</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0</v>
+      </c>
+      <c r="G13" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="54"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="17">
+        <v>1</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0</v>
+      </c>
+      <c r="G14" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="54"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="17">
+        <v>1</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0</v>
+      </c>
+      <c r="G15" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="54"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="19">
+      <c r="D16" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="17">
         <v>3</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="21">
+      <c r="F16" s="6">
+        <v>0</v>
+      </c>
+      <c r="G16" s="18">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="51"/>
-      <c r="B12" s="51"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="52"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="45" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="54"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="6">
+        <v>0</v>
+      </c>
+      <c r="G17" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="54"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="38">
+        <v>1</v>
+      </c>
+      <c r="F18" s="6">
+        <v>0</v>
+      </c>
+      <c r="G18" s="18">
+        <f t="shared" ref="G18:G19" si="1">E18-F18</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="54"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="38">
+        <v>3</v>
+      </c>
+      <c r="F19" s="6">
+        <v>0</v>
+      </c>
+      <c r="G19" s="18">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="54"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="17">
+        <v>1</v>
+      </c>
+      <c r="F20" s="6">
+        <v>0</v>
+      </c>
+      <c r="G20" s="18">
+        <f>E20-F20</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="54"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="17">
+        <v>2</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0</v>
+      </c>
+      <c r="G21" s="18">
+        <f>E21-F21</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="55"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="17">
+        <v>1</v>
+      </c>
+      <c r="F22" s="6">
+        <v>0</v>
+      </c>
+      <c r="G22" s="18">
+        <f>E22-F22</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="24"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="42">
+        <f>SUM(G5:G22)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="58"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="59"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="60"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="61"/>
+    </row>
+    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="68" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="50">
+        <f>SUM(E26:E37)</f>
+        <v>17</v>
+      </c>
+      <c r="C26" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="74">
+        <v>1</v>
+      </c>
+      <c r="F26" s="48">
+        <v>0</v>
+      </c>
+      <c r="G26" s="76">
+        <f>E26-F26</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="69"/>
+      <c r="B27" s="51"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="75"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="77"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="69"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="21">
+        <v>2</v>
+      </c>
+      <c r="F28" s="19">
+        <v>0</v>
+      </c>
+      <c r="G28" s="16">
+        <f t="shared" ref="G28:G53" si="2">E28-F28</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="69"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="17">
+        <v>1</v>
+      </c>
+      <c r="F29" s="7">
+        <v>0</v>
+      </c>
+      <c r="G29" s="16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="69"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="17">
+        <v>1</v>
+      </c>
+      <c r="F30" s="19">
+        <v>0</v>
+      </c>
+      <c r="G30" s="16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="69"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="17">
+        <v>2</v>
+      </c>
+      <c r="F31" s="7">
+        <v>0</v>
+      </c>
+      <c r="G31" s="16">
+        <f>E31-F31</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="69"/>
+      <c r="B32" s="51"/>
+      <c r="C32" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" s="17">
+        <v>2</v>
+      </c>
+      <c r="F32" s="19">
+        <v>0</v>
+      </c>
+      <c r="G32" s="16">
+        <f>E32-F32</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="69"/>
+      <c r="B33" s="51"/>
+      <c r="C33" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" s="17">
+        <v>1</v>
+      </c>
+      <c r="F33" s="7">
+        <v>0</v>
+      </c>
+      <c r="G33" s="16">
+        <f>E33-F33</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="69"/>
+      <c r="B34" s="51"/>
+      <c r="C34" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" s="17">
+        <v>3</v>
+      </c>
+      <c r="F34" s="19">
+        <v>0</v>
+      </c>
+      <c r="G34" s="16">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="69"/>
+      <c r="B35" s="51"/>
+      <c r="C35" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E35" s="17">
+        <v>1</v>
+      </c>
+      <c r="F35" s="7">
+        <v>0</v>
+      </c>
+      <c r="G35" s="16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="69"/>
+      <c r="B36" s="51"/>
+      <c r="C36" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36" s="17">
+        <v>2</v>
+      </c>
+      <c r="F36" s="19">
+        <v>0</v>
+      </c>
+      <c r="G36" s="16">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="69"/>
+      <c r="B37" s="51"/>
+      <c r="C37" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" s="20">
+        <v>1</v>
+      </c>
+      <c r="F37" s="7">
+        <v>0</v>
+      </c>
+      <c r="G37" s="22">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="33"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="41">
+        <f>SUM(G26:G37)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" s="73"/>
+      <c r="C39" s="73"/>
+      <c r="D39" s="73"/>
+      <c r="E39" s="73"/>
+      <c r="F39" s="73"/>
+      <c r="G39" s="59"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="60"/>
+      <c r="B40" s="60"/>
+      <c r="C40" s="60"/>
+      <c r="D40" s="60"/>
+      <c r="E40" s="60"/>
+      <c r="F40" s="60"/>
+      <c r="G40" s="61"/>
+    </row>
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="41"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="49"/>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="50"/>
-    </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
+      <c r="B41" s="50">
+        <f>SUM(E41:E55,4)</f>
+        <v>21</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" s="17">
+        <v>1</v>
+      </c>
+      <c r="F41" s="7">
+        <v>0</v>
+      </c>
+      <c r="G41" s="16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="71"/>
+      <c r="B42" s="51"/>
+      <c r="C42" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E42" s="17">
+        <v>2</v>
+      </c>
+      <c r="F42" s="7">
+        <v>0</v>
+      </c>
+      <c r="G42" s="16">
+        <f>E42-F42</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="71"/>
+      <c r="B43" s="51"/>
+      <c r="C43" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43" s="17">
+        <v>1</v>
+      </c>
+      <c r="F43" s="7">
+        <v>0</v>
+      </c>
+      <c r="G43" s="16">
+        <f>E43-F43</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="71"/>
+      <c r="B44" s="51"/>
+      <c r="C44" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E44" s="17">
+        <v>1</v>
+      </c>
+      <c r="F44" s="7">
+        <v>0</v>
+      </c>
+      <c r="G44" s="16">
+        <f>E44-F44</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="71"/>
+      <c r="B45" s="51"/>
+      <c r="C45" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E45" s="17">
+        <v>1</v>
+      </c>
+      <c r="F45" s="7">
+        <v>0</v>
+      </c>
+      <c r="G45" s="16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="71"/>
+      <c r="B46" s="51"/>
+      <c r="C46" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D46" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E46" s="17">
+        <v>1</v>
+      </c>
+      <c r="F46" s="7">
+        <v>0</v>
+      </c>
+      <c r="G46" s="16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="71"/>
+      <c r="B47" s="51"/>
+      <c r="C47" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E47" s="17">
+        <v>1</v>
+      </c>
+      <c r="F47" s="7">
+        <v>0</v>
+      </c>
+      <c r="G47" s="16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="71"/>
+      <c r="B48" s="51"/>
+      <c r="C48" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D48" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E48" s="17">
+        <v>1</v>
+      </c>
+      <c r="F48" s="7">
+        <v>0</v>
+      </c>
+      <c r="G48" s="16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="71"/>
+      <c r="B49" s="51"/>
+      <c r="C49" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D49" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E49" s="20">
+        <v>1</v>
+      </c>
+      <c r="F49" s="7">
+        <v>0</v>
+      </c>
+      <c r="G49" s="16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="71"/>
+      <c r="B50" s="51"/>
+      <c r="C50" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D50" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="E50" s="20">
+        <v>1</v>
+      </c>
+      <c r="F50" s="7">
+        <v>0</v>
+      </c>
+      <c r="G50" s="16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="71"/>
+      <c r="B51" s="51"/>
+      <c r="C51" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D51" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E51" s="20">
+        <v>2</v>
+      </c>
+      <c r="F51" s="7">
+        <v>0</v>
+      </c>
+      <c r="G51" s="16">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="71"/>
+      <c r="B52" s="51"/>
+      <c r="C52" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D52" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E52" s="20">
+        <v>1</v>
+      </c>
+      <c r="F52" s="7">
+        <v>0</v>
+      </c>
+      <c r="G52" s="16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="71"/>
+      <c r="B53" s="51"/>
+      <c r="C53" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D53" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="E53" s="20">
+        <v>2</v>
+      </c>
+      <c r="F53" s="7">
+        <v>0</v>
+      </c>
+      <c r="G53" s="16">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="72"/>
+      <c r="B54" s="51"/>
+      <c r="C54" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="D54" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="E54" s="46">
+        <v>1</v>
+      </c>
+      <c r="F54" s="7">
+        <v>0</v>
+      </c>
+      <c r="G54" s="16">
+        <f>E54-F54</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="15"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="43">
+        <f>SUM(G41:G54)</f>
         <v>17</v>
       </c>
-      <c r="B15" s="24">
-        <f>SUM(G15:G21)</f>
-        <v>13</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="53">
-        <v>2</v>
-      </c>
-      <c r="F15" s="22"/>
-      <c r="G15" s="55">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="56"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="19">
-        <v>1</v>
-      </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="18">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="39"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="19">
-        <v>1</v>
-      </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="18">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="39"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="19">
-        <v>4</v>
-      </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="18">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="39"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="19">
-        <v>2</v>
-      </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="18">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="39"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E21" s="19">
-        <v>3</v>
-      </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="18">
-        <f t="shared" ref="G21" si="1">E21-F21</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="40"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="41"/>
-    </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="45" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="46"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="48"/>
-    </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="24">
-        <f>SUM(E25:E31,4)</f>
-        <v>19.5</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="19">
-        <v>2</v>
-      </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="18">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="43"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" s="19">
-        <v>1</v>
-      </c>
-      <c r="F26" s="7"/>
-      <c r="G26" s="18">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="43"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="18">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="43"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" s="19">
-        <v>6</v>
-      </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="18">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="43"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E29" s="19">
-        <v>4</v>
-      </c>
-      <c r="F29" s="7"/>
-      <c r="G29" s="18">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="44"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E30" s="20">
-        <v>2</v>
-      </c>
-      <c r="F30" s="8"/>
-      <c r="G30" s="18">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="17">
-        <f ca="1">SUM(G25:G31,G5:G11,G15:G21)</f>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="11"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="44">
+        <f ca="1">SUM(G41:G56,G5:G22,G26:G37)</f>
         <v>48.5</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="H32" s="12"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
-      <c r="H43" s="12"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-      <c r="H46" s="12"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-      <c r="H47" s="12"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-      <c r="H48" s="12"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="12"/>
-      <c r="B49" s="12"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
-      <c r="H49" s="12"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="12"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="12"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="12"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
-      <c r="H51" s="12"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="12"/>
-      <c r="B52" s="12"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="12"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="12"/>
-      <c r="B53" s="12"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
-      <c r="H53" s="12"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="12"/>
-      <c r="B54" s="12"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
-      <c r="H54" s="12"/>
+      <c r="H56" s="11"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="11"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="11"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="11"/>
+      <c r="B59" s="11"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="11"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="11"/>
+      <c r="B61" s="11"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="11"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="11"/>
+      <c r="B62" s="11"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="11"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="11"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="11"/>
+      <c r="B65" s="11"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="11"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="11"/>
+      <c r="B67" s="11"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="11"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="11"/>
+      <c r="B68" s="11"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="11"/>
+      <c r="G68" s="11"/>
+      <c r="H68" s="11"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="11"/>
+      <c r="B69" s="11"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+      <c r="H69" s="11"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="11"/>
+      <c r="B70" s="11"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="12"/>
+      <c r="E70" s="11"/>
+      <c r="F70" s="11"/>
+      <c r="G70" s="11"/>
+      <c r="H70" s="11"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="11"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="11"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="11"/>
+      <c r="B72" s="11"/>
+      <c r="C72" s="11"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
+      <c r="G72" s="11"/>
+      <c r="H72" s="11"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="11"/>
+      <c r="B73" s="11"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="11"/>
+      <c r="F73" s="11"/>
+      <c r="G73" s="11"/>
+      <c r="H73" s="11"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="11"/>
+      <c r="B74" s="11"/>
+      <c r="C74" s="11"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="11"/>
+      <c r="F74" s="11"/>
+      <c r="G74" s="11"/>
+      <c r="H74" s="11"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="11"/>
+      <c r="B75" s="11"/>
+      <c r="C75" s="11"/>
+      <c r="D75" s="12"/>
+      <c r="E75" s="11"/>
+      <c r="F75" s="11"/>
+      <c r="G75" s="11"/>
+      <c r="H75" s="11"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="11"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="11"/>
+      <c r="F76" s="11"/>
+      <c r="G76" s="13"/>
+      <c r="H76" s="11"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="11"/>
+      <c r="B77" s="11"/>
+      <c r="C77" s="11"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="11"/>
+      <c r="F77" s="11"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="11"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="11"/>
+      <c r="B78" s="11"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="11"/>
+      <c r="F78" s="11"/>
+      <c r="G78" s="11"/>
+      <c r="H78" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="19">
     <mergeCell ref="A3:G4"/>
-    <mergeCell ref="B15:B21"/>
-    <mergeCell ref="A15:A21"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="B25:B30"/>
-    <mergeCell ref="A25:A30"/>
-    <mergeCell ref="A23:G24"/>
-    <mergeCell ref="A13:G14"/>
-    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="B26:B37"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B41:B54"/>
+    <mergeCell ref="A41:A54"/>
+    <mergeCell ref="A39:G40"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="G5:G6"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B5:B11"/>
-    <mergeCell ref="A5:A11"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="B5:B22"/>
+    <mergeCell ref="A5:A22"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="A24:G25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Author : Rachit Goyal File Modified : RachitGoyal.xlsx Description : Time Update
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/RachitGoyal.xlsx
+++ b/TeamDetails/TasksBreakDown/RachitGoyal.xlsx
@@ -53,7 +53,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Time estimation for the above Story.</t>
+Remaining Time for the above Story.</t>
         </r>
       </text>
     </comment>
@@ -77,7 +77,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Time estimation for the above Story.</t>
+Remainig Time for the above Story.</t>
         </r>
       </text>
     </comment>
@@ -101,7 +101,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Time estimation for the above Story.</t>
+Remaining Time for the above Story.</t>
         </r>
       </text>
     </comment>
@@ -216,32 +216,6 @@
   </si>
   <si>
     <r>
-      <t>Create a Downlaod</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Button</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.(certificate)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Create a </t>
     </r>
     <r>
@@ -865,6 +839,32 @@
         <scheme val="minor"/>
       </rPr>
       <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Create a Download</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Button</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.(certificate)</t>
     </r>
   </si>
 </sst>
@@ -1397,17 +1397,56 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1430,15 +1469,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1462,36 +1492,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1782,8 +1782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="I60" sqref="I60"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1820,67 +1820,67 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="64"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="74"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="65"/>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="67"/>
+      <c r="A4" s="75"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="77"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="50">
+      <c r="B5" s="48">
         <f>SUM(E5:E22)</f>
         <v>23</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="78" t="s">
+      <c r="D5" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="74">
-        <v>1</v>
-      </c>
-      <c r="F5" s="48">
-        <v>0</v>
-      </c>
-      <c r="G5" s="76">
+      <c r="E5" s="57">
+        <v>1</v>
+      </c>
+      <c r="F5" s="59">
+        <v>0</v>
+      </c>
+      <c r="G5" s="61">
         <f>E5-F5</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="54"/>
-      <c r="B6" s="51"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="77"/>
+      <c r="A6" s="67"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="62"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="54"/>
-      <c r="B7" s="51"/>
+      <c r="A7" s="67"/>
+      <c r="B7" s="49"/>
       <c r="C7" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="21">
         <v>2</v>
@@ -1894,13 +1894,13 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="54"/>
-      <c r="B8" s="51"/>
+      <c r="A8" s="67"/>
+      <c r="B8" s="49"/>
       <c r="C8" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" s="17">
         <v>1</v>
@@ -1914,13 +1914,13 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="54"/>
-      <c r="B9" s="51"/>
+      <c r="A9" s="67"/>
+      <c r="B9" s="49"/>
       <c r="C9" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E9" s="17">
         <v>1</v>
@@ -1934,13 +1934,13 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="54"/>
-      <c r="B10" s="51"/>
+      <c r="A10" s="67"/>
+      <c r="B10" s="49"/>
       <c r="C10" s="25" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" s="17">
         <v>1</v>
@@ -1954,113 +1954,113 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="54"/>
-      <c r="B11" s="51"/>
+      <c r="A11" s="67"/>
+      <c r="B11" s="49"/>
       <c r="C11" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="17">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0</v>
+      </c>
+      <c r="G11" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="67"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="17">
-        <v>1</v>
-      </c>
-      <c r="F11" s="6">
-        <v>0</v>
-      </c>
-      <c r="G11" s="18">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="54"/>
-      <c r="B12" s="51"/>
-      <c r="C12" s="6" t="s">
+      <c r="E12" s="17">
+        <v>1</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0</v>
+      </c>
+      <c r="G12" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="67"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D13" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="17">
-        <v>1</v>
-      </c>
-      <c r="F12" s="6">
-        <v>0</v>
-      </c>
-      <c r="G12" s="18">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="54"/>
-      <c r="B13" s="51"/>
-      <c r="C13" s="25" t="s">
+      <c r="E13" s="17">
+        <v>1</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0</v>
+      </c>
+      <c r="G13" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="67"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D14" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="17">
-        <v>1</v>
-      </c>
-      <c r="F13" s="6">
-        <v>0</v>
-      </c>
-      <c r="G13" s="18">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="54"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="6" t="s">
+      <c r="E14" s="17">
+        <v>1</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0</v>
+      </c>
+      <c r="G14" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="67"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D15" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="17">
-        <v>1</v>
-      </c>
-      <c r="F14" s="6">
-        <v>0</v>
-      </c>
-      <c r="G14" s="18">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="54"/>
-      <c r="B15" s="51"/>
-      <c r="C15" s="6" t="s">
+      <c r="E15" s="17">
+        <v>1</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0</v>
+      </c>
+      <c r="G15" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="67"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D16" s="26" t="s">
         <v>39</v>
-      </c>
-      <c r="E15" s="17">
-        <v>1</v>
-      </c>
-      <c r="F15" s="6">
-        <v>0</v>
-      </c>
-      <c r="G15" s="18">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="54"/>
-      <c r="B16" s="51"/>
-      <c r="C16" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="26" t="s">
-        <v>40</v>
       </c>
       <c r="E16" s="17">
         <v>3</v>
@@ -2074,33 +2074,33 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="54"/>
-      <c r="B17" s="51"/>
+      <c r="A17" s="67"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="6">
+        <v>0</v>
+      </c>
+      <c r="G17" s="18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="67"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="17">
-        <v>1</v>
-      </c>
-      <c r="F17" s="6">
-        <v>0</v>
-      </c>
-      <c r="G17" s="18">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="54"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="6" t="s">
-        <v>32</v>
-      </c>
       <c r="D18" s="40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E18" s="38">
         <v>1</v>
@@ -2114,13 +2114,13 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="54"/>
-      <c r="B19" s="51"/>
+      <c r="A19" s="67"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D19" s="40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E19" s="38">
         <v>3</v>
@@ -2134,13 +2134,13 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="54"/>
-      <c r="B20" s="51"/>
+      <c r="A20" s="67"/>
+      <c r="B20" s="49"/>
       <c r="C20" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D20" s="39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E20" s="17">
         <v>1</v>
@@ -2154,13 +2154,13 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="54"/>
-      <c r="B21" s="51"/>
+      <c r="A21" s="67"/>
+      <c r="B21" s="49"/>
       <c r="C21" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E21" s="17">
         <v>2</v>
@@ -2174,13 +2174,13 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="55"/>
-      <c r="B22" s="52"/>
+      <c r="A22" s="68"/>
+      <c r="B22" s="65"/>
       <c r="C22" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E22" s="17">
         <v>1</v>
@@ -2206,107 +2206,107 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="58" t="s">
+      <c r="A24" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="58"/>
-      <c r="C24" s="58"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="58"/>
-      <c r="F24" s="58"/>
-      <c r="G24" s="59"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="54"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="60"/>
-      <c r="B25" s="60"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="61"/>
+      <c r="A25" s="55"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="56"/>
     </row>
     <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="68" t="s">
+      <c r="A26" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="50">
+      <c r="B26" s="48">
         <f>SUM(E26:E37)</f>
         <v>17</v>
       </c>
-      <c r="C26" s="48" t="s">
+      <c r="C26" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="56" t="s">
+      <c r="D26" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="74">
-        <v>1</v>
-      </c>
-      <c r="F26" s="48">
-        <v>0</v>
-      </c>
-      <c r="G26" s="76">
+      <c r="E26" s="57">
+        <v>1</v>
+      </c>
+      <c r="F26" s="59">
+        <v>1</v>
+      </c>
+      <c r="G26" s="61">
         <f>E26-F26</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="69"/>
-      <c r="B27" s="51"/>
-      <c r="C27" s="49"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="77"/>
+      <c r="A27" s="79"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="62"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="69"/>
-      <c r="B28" s="51"/>
+      <c r="A28" s="79"/>
+      <c r="B28" s="49"/>
       <c r="C28" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E28" s="21">
         <v>2</v>
       </c>
       <c r="F28" s="19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G28" s="16">
         <f t="shared" ref="G28:G53" si="2">E28-F28</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="69"/>
-      <c r="B29" s="51"/>
+      <c r="A29" s="79"/>
+      <c r="B29" s="49"/>
       <c r="C29" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E29" s="17">
         <v>1</v>
       </c>
       <c r="F29" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" s="16">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="69"/>
-      <c r="B30" s="51"/>
+      <c r="A30" s="79"/>
+      <c r="B30" s="49"/>
       <c r="C30" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="E30" s="17">
         <v>1</v>
@@ -2320,13 +2320,13 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="69"/>
-      <c r="B31" s="51"/>
+      <c r="A31" s="79"/>
+      <c r="B31" s="49"/>
       <c r="C31" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E31" s="17">
         <v>2</v>
@@ -2340,13 +2340,13 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="69"/>
-      <c r="B32" s="51"/>
+      <c r="A32" s="79"/>
+      <c r="B32" s="49"/>
       <c r="C32" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E32" s="17">
         <v>2</v>
@@ -2360,33 +2360,33 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="69"/>
-      <c r="B33" s="51"/>
+      <c r="A33" s="79"/>
+      <c r="B33" s="49"/>
       <c r="C33" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E33" s="17">
         <v>1</v>
       </c>
       <c r="F33" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33" s="16">
         <f>E33-F33</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="69"/>
-      <c r="B34" s="51"/>
+      <c r="A34" s="79"/>
+      <c r="B34" s="49"/>
       <c r="C34" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E34" s="17">
         <v>3</v>
@@ -2400,13 +2400,13 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="69"/>
-      <c r="B35" s="51"/>
+      <c r="A35" s="79"/>
+      <c r="B35" s="49"/>
       <c r="C35" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D35" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E35" s="17">
         <v>1</v>
@@ -2420,13 +2420,13 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="69"/>
-      <c r="B36" s="51"/>
+      <c r="A36" s="79"/>
+      <c r="B36" s="49"/>
       <c r="C36" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E36" s="17">
         <v>2</v>
@@ -2440,13 +2440,13 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="69"/>
-      <c r="B37" s="51"/>
+      <c r="A37" s="79"/>
+      <c r="B37" s="49"/>
       <c r="C37" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D37" s="31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E37" s="20">
         <v>1</v>
@@ -2468,34 +2468,34 @@
       <c r="F38" s="32"/>
       <c r="G38" s="41">
         <f>SUM(G26:G37)</f>
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="73" t="s">
+      <c r="A39" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="B39" s="73"/>
-      <c r="C39" s="73"/>
-      <c r="D39" s="73"/>
-      <c r="E39" s="73"/>
-      <c r="F39" s="73"/>
-      <c r="G39" s="59"/>
+      <c r="B39" s="53"/>
+      <c r="C39" s="53"/>
+      <c r="D39" s="53"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="53"/>
+      <c r="G39" s="54"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="60"/>
-      <c r="B40" s="60"/>
-      <c r="C40" s="60"/>
-      <c r="D40" s="60"/>
-      <c r="E40" s="60"/>
-      <c r="F40" s="60"/>
-      <c r="G40" s="61"/>
+      <c r="A40" s="55"/>
+      <c r="B40" s="55"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="55"/>
+      <c r="E40" s="55"/>
+      <c r="F40" s="55"/>
+      <c r="G40" s="56"/>
     </row>
     <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="70" t="s">
+      <c r="A41" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="50">
+      <c r="B41" s="48">
         <f>SUM(E41:E55,4)</f>
         <v>21</v>
       </c>
@@ -2517,13 +2517,13 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="71"/>
-      <c r="B42" s="51"/>
+      <c r="A42" s="51"/>
+      <c r="B42" s="49"/>
       <c r="C42" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E42" s="17">
         <v>2</v>
@@ -2537,8 +2537,8 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="71"/>
-      <c r="B43" s="51"/>
+      <c r="A43" s="51"/>
+      <c r="B43" s="49"/>
       <c r="C43" s="7" t="s">
         <v>7</v>
       </c>
@@ -2557,13 +2557,13 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="71"/>
-      <c r="B44" s="51"/>
+      <c r="A44" s="51"/>
+      <c r="B44" s="49"/>
       <c r="C44" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E44" s="17">
         <v>1</v>
@@ -2577,13 +2577,13 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="71"/>
-      <c r="B45" s="51"/>
+      <c r="A45" s="51"/>
+      <c r="B45" s="49"/>
       <c r="C45" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E45" s="17">
         <v>1</v>
@@ -2597,13 +2597,13 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="71"/>
-      <c r="B46" s="51"/>
+      <c r="A46" s="51"/>
+      <c r="B46" s="49"/>
       <c r="C46" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E46" s="17">
         <v>1</v>
@@ -2617,13 +2617,13 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="71"/>
-      <c r="B47" s="51"/>
+      <c r="A47" s="51"/>
+      <c r="B47" s="49"/>
       <c r="C47" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D47" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E47" s="17">
         <v>1</v>
@@ -2637,13 +2637,13 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="71"/>
-      <c r="B48" s="51"/>
+      <c r="A48" s="51"/>
+      <c r="B48" s="49"/>
       <c r="C48" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E48" s="17">
         <v>1</v>
@@ -2657,13 +2657,13 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="71"/>
-      <c r="B49" s="51"/>
+      <c r="A49" s="51"/>
+      <c r="B49" s="49"/>
       <c r="C49" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D49" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E49" s="20">
         <v>1</v>
@@ -2677,13 +2677,13 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="71"/>
-      <c r="B50" s="51"/>
+      <c r="A50" s="51"/>
+      <c r="B50" s="49"/>
       <c r="C50" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D50" s="26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E50" s="20">
         <v>1</v>
@@ -2697,13 +2697,13 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="71"/>
-      <c r="B51" s="51"/>
+      <c r="A51" s="51"/>
+      <c r="B51" s="49"/>
       <c r="C51" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D51" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E51" s="20">
         <v>2</v>
@@ -2717,13 +2717,13 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="71"/>
-      <c r="B52" s="51"/>
+      <c r="A52" s="51"/>
+      <c r="B52" s="49"/>
       <c r="C52" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D52" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E52" s="20">
         <v>1</v>
@@ -2737,13 +2737,13 @@
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="71"/>
-      <c r="B53" s="51"/>
+      <c r="A53" s="51"/>
+      <c r="B53" s="49"/>
       <c r="C53" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D53" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E53" s="20">
         <v>2</v>
@@ -2757,13 +2757,13 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="72"/>
-      <c r="B54" s="51"/>
+      <c r="A54" s="52"/>
+      <c r="B54" s="49"/>
       <c r="C54" s="45" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D54" s="47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E54" s="46">
         <v>1</v>

</xml_diff>

<commit_message>
Author : Rachit Goyal File Modified : RachitGoyal.xlsx
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/RachitGoyal.xlsx
+++ b/TeamDetails/TasksBreakDown/RachitGoyal.xlsx
@@ -1397,12 +1397,36 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1468,30 +1492,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1782,8 +1782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1820,62 +1820,62 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="74"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="50"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="75"/>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="77"/>
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="53"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="48">
+      <c r="B5" s="54">
         <f>SUM(E5:E22)</f>
         <v>23</v>
       </c>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="63" t="s">
+      <c r="D5" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="57">
-        <v>1</v>
-      </c>
-      <c r="F5" s="59">
-        <v>0</v>
-      </c>
-      <c r="G5" s="61">
+      <c r="E5" s="65">
+        <v>1</v>
+      </c>
+      <c r="F5" s="67">
+        <v>1</v>
+      </c>
+      <c r="G5" s="69">
         <f>E5-F5</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="67"/>
-      <c r="B6" s="49"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="62"/>
+      <c r="A6" s="75"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="70"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="67"/>
-      <c r="B7" s="49"/>
+      <c r="A7" s="75"/>
+      <c r="B7" s="55"/>
       <c r="C7" s="6" t="s">
         <v>9</v>
       </c>
@@ -1886,16 +1886,16 @@
         <v>2</v>
       </c>
       <c r="F7" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="18">
         <f t="shared" ref="G7:G17" si="0">E7-F7</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="67"/>
-      <c r="B8" s="49"/>
+      <c r="A8" s="75"/>
+      <c r="B8" s="55"/>
       <c r="C8" s="6" t="s">
         <v>7</v>
       </c>
@@ -1906,16 +1906,16 @@
         <v>1</v>
       </c>
       <c r="F8" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="18">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="67"/>
-      <c r="B9" s="49"/>
+      <c r="A9" s="75"/>
+      <c r="B9" s="55"/>
       <c r="C9" s="6" t="s">
         <v>8</v>
       </c>
@@ -1934,8 +1934,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="67"/>
-      <c r="B10" s="49"/>
+      <c r="A10" s="75"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="25" t="s">
         <v>10</v>
       </c>
@@ -1954,8 +1954,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="67"/>
-      <c r="B11" s="49"/>
+      <c r="A11" s="75"/>
+      <c r="B11" s="55"/>
       <c r="C11" s="6" t="s">
         <v>12</v>
       </c>
@@ -1974,8 +1974,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="67"/>
-      <c r="B12" s="49"/>
+      <c r="A12" s="75"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="6" t="s">
         <v>25</v>
       </c>
@@ -1994,8 +1994,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="67"/>
-      <c r="B13" s="49"/>
+      <c r="A13" s="75"/>
+      <c r="B13" s="55"/>
       <c r="C13" s="25" t="s">
         <v>26</v>
       </c>
@@ -2014,8 +2014,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="67"/>
-      <c r="B14" s="49"/>
+      <c r="A14" s="75"/>
+      <c r="B14" s="55"/>
       <c r="C14" s="6" t="s">
         <v>27</v>
       </c>
@@ -2034,8 +2034,8 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="67"/>
-      <c r="B15" s="49"/>
+      <c r="A15" s="75"/>
+      <c r="B15" s="55"/>
       <c r="C15" s="6" t="s">
         <v>28</v>
       </c>
@@ -2054,8 +2054,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="67"/>
-      <c r="B16" s="49"/>
+      <c r="A16" s="75"/>
+      <c r="B16" s="55"/>
       <c r="C16" s="25" t="s">
         <v>29</v>
       </c>
@@ -2074,8 +2074,8 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="67"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="75"/>
+      <c r="B17" s="55"/>
       <c r="C17" s="6" t="s">
         <v>30</v>
       </c>
@@ -2094,8 +2094,8 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="67"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="75"/>
+      <c r="B18" s="55"/>
       <c r="C18" s="6" t="s">
         <v>31</v>
       </c>
@@ -2114,8 +2114,8 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="67"/>
-      <c r="B19" s="49"/>
+      <c r="A19" s="75"/>
+      <c r="B19" s="55"/>
       <c r="C19" s="6" t="s">
         <v>32</v>
       </c>
@@ -2134,8 +2134,8 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="67"/>
-      <c r="B20" s="49"/>
+      <c r="A20" s="75"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="6" t="s">
         <v>46</v>
       </c>
@@ -2154,8 +2154,8 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="67"/>
-      <c r="B21" s="49"/>
+      <c r="A21" s="75"/>
+      <c r="B21" s="55"/>
       <c r="C21" s="6" t="s">
         <v>47</v>
       </c>
@@ -2174,8 +2174,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="68"/>
-      <c r="B22" s="65"/>
+      <c r="A22" s="76"/>
+      <c r="B22" s="73"/>
       <c r="C22" s="6" t="s">
         <v>48</v>
       </c>
@@ -2202,66 +2202,66 @@
       <c r="F23" s="24"/>
       <c r="G23" s="42">
         <f>SUM(G5:G22)</f>
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="71" t="s">
+      <c r="A24" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="71"/>
-      <c r="C24" s="71"/>
-      <c r="D24" s="71"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="54"/>
+      <c r="B24" s="79"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="79"/>
+      <c r="E24" s="79"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="62"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="55"/>
-      <c r="B25" s="55"/>
-      <c r="C25" s="55"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="56"/>
+      <c r="A25" s="63"/>
+      <c r="B25" s="63"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="63"/>
+      <c r="F25" s="63"/>
+      <c r="G25" s="64"/>
     </row>
     <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="78" t="s">
+      <c r="A26" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="48">
+      <c r="B26" s="54">
         <f>SUM(E26:E37)</f>
         <v>17</v>
       </c>
-      <c r="C26" s="59" t="s">
+      <c r="C26" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="69" t="s">
+      <c r="D26" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="57">
-        <v>1</v>
-      </c>
-      <c r="F26" s="59">
-        <v>1</v>
-      </c>
-      <c r="G26" s="61">
+      <c r="E26" s="65">
+        <v>1</v>
+      </c>
+      <c r="F26" s="67">
+        <v>1</v>
+      </c>
+      <c r="G26" s="69">
         <f>E26-F26</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="79"/>
-      <c r="B27" s="49"/>
-      <c r="C27" s="60"/>
-      <c r="D27" s="70"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="60"/>
-      <c r="G27" s="62"/>
+      <c r="A27" s="57"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="78"/>
+      <c r="E27" s="66"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="70"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="79"/>
-      <c r="B28" s="49"/>
+      <c r="A28" s="57"/>
+      <c r="B28" s="55"/>
       <c r="C28" s="6" t="s">
         <v>9</v>
       </c>
@@ -2280,8 +2280,8 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="79"/>
-      <c r="B29" s="49"/>
+      <c r="A29" s="57"/>
+      <c r="B29" s="55"/>
       <c r="C29" s="6" t="s">
         <v>7</v>
       </c>
@@ -2300,8 +2300,8 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="79"/>
-      <c r="B30" s="49"/>
+      <c r="A30" s="57"/>
+      <c r="B30" s="55"/>
       <c r="C30" s="6" t="s">
         <v>8</v>
       </c>
@@ -2312,16 +2312,16 @@
         <v>1</v>
       </c>
       <c r="F30" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" s="16">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="79"/>
-      <c r="B31" s="49"/>
+      <c r="A31" s="57"/>
+      <c r="B31" s="55"/>
       <c r="C31" s="6" t="s">
         <v>10</v>
       </c>
@@ -2340,8 +2340,8 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="79"/>
-      <c r="B32" s="49"/>
+      <c r="A32" s="57"/>
+      <c r="B32" s="55"/>
       <c r="C32" s="6" t="s">
         <v>12</v>
       </c>
@@ -2360,8 +2360,8 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="79"/>
-      <c r="B33" s="49"/>
+      <c r="A33" s="57"/>
+      <c r="B33" s="55"/>
       <c r="C33" s="6" t="s">
         <v>25</v>
       </c>
@@ -2380,8 +2380,8 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="79"/>
-      <c r="B34" s="49"/>
+      <c r="A34" s="57"/>
+      <c r="B34" s="55"/>
       <c r="C34" s="6" t="s">
         <v>26</v>
       </c>
@@ -2400,8 +2400,8 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="79"/>
-      <c r="B35" s="49"/>
+      <c r="A35" s="57"/>
+      <c r="B35" s="55"/>
       <c r="C35" s="6" t="s">
         <v>27</v>
       </c>
@@ -2420,8 +2420,8 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="79"/>
-      <c r="B36" s="49"/>
+      <c r="A36" s="57"/>
+      <c r="B36" s="55"/>
       <c r="C36" s="6" t="s">
         <v>28</v>
       </c>
@@ -2440,8 +2440,8 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="79"/>
-      <c r="B37" s="49"/>
+      <c r="A37" s="57"/>
+      <c r="B37" s="55"/>
       <c r="C37" s="30" t="s">
         <v>29</v>
       </c>
@@ -2468,34 +2468,34 @@
       <c r="F38" s="32"/>
       <c r="G38" s="41">
         <f>SUM(G26:G37)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="53" t="s">
+      <c r="A39" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="B39" s="53"/>
-      <c r="C39" s="53"/>
-      <c r="D39" s="53"/>
-      <c r="E39" s="53"/>
-      <c r="F39" s="53"/>
-      <c r="G39" s="54"/>
+      <c r="B39" s="61"/>
+      <c r="C39" s="61"/>
+      <c r="D39" s="61"/>
+      <c r="E39" s="61"/>
+      <c r="F39" s="61"/>
+      <c r="G39" s="62"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="55"/>
-      <c r="B40" s="55"/>
-      <c r="C40" s="55"/>
-      <c r="D40" s="55"/>
-      <c r="E40" s="55"/>
-      <c r="F40" s="55"/>
-      <c r="G40" s="56"/>
+      <c r="A40" s="63"/>
+      <c r="B40" s="63"/>
+      <c r="C40" s="63"/>
+      <c r="D40" s="63"/>
+      <c r="E40" s="63"/>
+      <c r="F40" s="63"/>
+      <c r="G40" s="64"/>
     </row>
     <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="50" t="s">
+      <c r="A41" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="48">
+      <c r="B41" s="54">
         <f>SUM(E41:E55,4)</f>
         <v>21</v>
       </c>
@@ -2509,16 +2509,16 @@
         <v>1</v>
       </c>
       <c r="F41" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41" s="16">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="51"/>
-      <c r="B42" s="49"/>
+      <c r="A42" s="59"/>
+      <c r="B42" s="55"/>
       <c r="C42" s="7" t="s">
         <v>9</v>
       </c>
@@ -2529,16 +2529,16 @@
         <v>2</v>
       </c>
       <c r="F42" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G42" s="16">
         <f>E42-F42</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="51"/>
-      <c r="B43" s="49"/>
+      <c r="A43" s="59"/>
+      <c r="B43" s="55"/>
       <c r="C43" s="7" t="s">
         <v>7</v>
       </c>
@@ -2549,16 +2549,16 @@
         <v>1</v>
       </c>
       <c r="F43" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" s="16">
         <f>E43-F43</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="51"/>
-      <c r="B44" s="49"/>
+      <c r="A44" s="59"/>
+      <c r="B44" s="55"/>
       <c r="C44" s="7" t="s">
         <v>8</v>
       </c>
@@ -2577,8 +2577,8 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="51"/>
-      <c r="B45" s="49"/>
+      <c r="A45" s="59"/>
+      <c r="B45" s="55"/>
       <c r="C45" s="7" t="s">
         <v>10</v>
       </c>
@@ -2597,8 +2597,8 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="51"/>
-      <c r="B46" s="49"/>
+      <c r="A46" s="59"/>
+      <c r="B46" s="55"/>
       <c r="C46" s="7" t="s">
         <v>12</v>
       </c>
@@ -2617,8 +2617,8 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="51"/>
-      <c r="B47" s="49"/>
+      <c r="A47" s="59"/>
+      <c r="B47" s="55"/>
       <c r="C47" s="7" t="s">
         <v>25</v>
       </c>
@@ -2637,8 +2637,8 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="51"/>
-      <c r="B48" s="49"/>
+      <c r="A48" s="59"/>
+      <c r="B48" s="55"/>
       <c r="C48" s="7" t="s">
         <v>26</v>
       </c>
@@ -2657,8 +2657,8 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="51"/>
-      <c r="B49" s="49"/>
+      <c r="A49" s="59"/>
+      <c r="B49" s="55"/>
       <c r="C49" s="7" t="s">
         <v>27</v>
       </c>
@@ -2677,8 +2677,8 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="51"/>
-      <c r="B50" s="49"/>
+      <c r="A50" s="59"/>
+      <c r="B50" s="55"/>
       <c r="C50" s="7" t="s">
         <v>28</v>
       </c>
@@ -2697,8 +2697,8 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="51"/>
-      <c r="B51" s="49"/>
+      <c r="A51" s="59"/>
+      <c r="B51" s="55"/>
       <c r="C51" s="7" t="s">
         <v>29</v>
       </c>
@@ -2717,8 +2717,8 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="51"/>
-      <c r="B52" s="49"/>
+      <c r="A52" s="59"/>
+      <c r="B52" s="55"/>
       <c r="C52" s="7" t="s">
         <v>30</v>
       </c>
@@ -2737,8 +2737,8 @@
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="51"/>
-      <c r="B53" s="49"/>
+      <c r="A53" s="59"/>
+      <c r="B53" s="55"/>
       <c r="C53" s="7" t="s">
         <v>31</v>
       </c>
@@ -2757,8 +2757,8 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="52"/>
-      <c r="B54" s="49"/>
+      <c r="A54" s="60"/>
+      <c r="B54" s="55"/>
       <c r="C54" s="45" t="s">
         <v>32</v>
       </c>
@@ -2784,7 +2784,7 @@
       <c r="F55" s="14"/>
       <c r="G55" s="43">
         <f>SUM(G41:G54)</f>
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -3022,6 +3022,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="A24:G25"/>
     <mergeCell ref="A3:G4"/>
     <mergeCell ref="B26:B37"/>
     <mergeCell ref="A26:A37"/>
@@ -3038,9 +3041,6 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="B5:B22"/>
     <mergeCell ref="A5:A22"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="A24:G25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>